<commit_message>
Tried constrained PRIM, works
</commit_message>
<xml_diff>
--- a/parsed_scenarios.xlsx
+++ b/parsed_scenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oscarste\OneDrive - Chalmers\Local files\Python repos\BECCS-Sweden\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197A478F-982A-423D-9574-5B558D4A1826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40050F42-C467-4346-B773-1524248BE2AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="58290" yWindow="2520" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
     <t>time</t>
   </si>
   <si>
-    <t>4692.553052</t>
+    <t>5375.493591</t>
   </si>
   <si>
     <t>5996.392208</t>
@@ -64,7 +64,7 @@
     <t>CHP2</t>
   </si>
   <si>
-    <t>4539.922962</t>
+    <t>5227.175586</t>
   </si>
   <si>
     <t>5997.172835</t>
@@ -73,13 +73,13 @@
     <t>CHP3</t>
   </si>
   <si>
+    <t>5373.471119</t>
+  </si>
+  <si>
+    <t>5999.593822</t>
+  </si>
+  <si>
     <t>1000</t>
-  </si>
-  <si>
-    <t>4540.717407</t>
-  </si>
-  <si>
-    <t>5999.593822</t>
   </si>
 </sst>
 </file>
@@ -445,7 +445,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,10 +525,13 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -536,13 +539,10 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -550,10 +550,13 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -561,13 +564,10 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>17</v>
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -575,10 +575,10 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
SD works for new CHP and W2E :)
</commit_message>
<xml_diff>
--- a/parsed_scenarios.xlsx
+++ b/parsed_scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oscarste\OneDrive - Chalmers\Local files\Python repos\BECCS-Sweden\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40050F42-C467-4346-B773-1524248BE2AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F695184-44BC-47D0-85BD-FCAEC95817D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58290" yWindow="2520" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="58">
   <si>
     <t>Scenario</t>
   </si>
@@ -40,6 +40,15 @@
     <t>CHP1</t>
   </si>
   <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>5381.821422</t>
+  </si>
+  <si>
+    <t>5996.392208</t>
+  </si>
+  <si>
     <t>duration_increase</t>
   </si>
   <si>
@@ -49,37 +58,142 @@
     <t>heat_pump</t>
   </si>
   <si>
+    <t>1.536347e-58</t>
+  </si>
+  <si>
     <t>{True}       {True}</t>
   </si>
   <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>5375.493591</t>
-  </si>
-  <si>
-    <t>5996.392208</t>
-  </si>
-  <si>
     <t>CHP2</t>
   </si>
   <si>
-    <t>5227.175586</t>
+    <t>i</t>
+  </si>
+  <si>
+    <t>0.050039</t>
+  </si>
+  <si>
+    <t>0.077334</t>
+  </si>
+  <si>
+    <t>5216.036943</t>
   </si>
   <si>
     <t>5997.172835</t>
   </si>
   <si>
+    <t>1000.000000</t>
+  </si>
+  <si>
     <t>CHP3</t>
   </si>
   <si>
-    <t>5373.471119</t>
+    <t>0.050007</t>
+  </si>
+  <si>
+    <t>0.074952</t>
+  </si>
+  <si>
+    <t>5156.961639</t>
   </si>
   <si>
     <t>5999.593822</t>
   </si>
   <si>
-    <t>1000</t>
+    <t>CHP11</t>
+  </si>
+  <si>
+    <t>1.387871e-22</t>
+  </si>
+  <si>
+    <t>{True}     {True}</t>
+  </si>
+  <si>
+    <t>COP</t>
+  </si>
+  <si>
+    <t>3.259885</t>
+  </si>
+  <si>
+    <t>3.698761</t>
+  </si>
+  <si>
+    <t>4841.663162</t>
+  </si>
+  <si>
+    <t>5994.3291</t>
+  </si>
+  <si>
+    <t>CHP22</t>
+  </si>
+  <si>
+    <t>9.520002e-17</t>
+  </si>
+  <si>
+    <t>celc</t>
+  </si>
+  <si>
+    <t>23.718479</t>
+  </si>
+  <si>
+    <t>65.499006</t>
+  </si>
+  <si>
+    <t>CHP33</t>
+  </si>
+  <si>
+    <t>0.066644</t>
+  </si>
+  <si>
+    <t>1.436419e-177</t>
+  </si>
+  <si>
+    <t>4986.332828</t>
+  </si>
+  <si>
+    <t>WASTE1</t>
+  </si>
+  <si>
+    <t>20.212437</t>
+  </si>
+  <si>
+    <t>80.944133</t>
+  </si>
+  <si>
+    <t>2.985703</t>
+  </si>
+  <si>
+    <t>3.796962</t>
+  </si>
+  <si>
+    <t>WASTE2</t>
+  </si>
+  <si>
+    <t>20.035578</t>
+  </si>
+  <si>
+    <t>74.087937</t>
+  </si>
+  <si>
+    <t>0.052697</t>
+  </si>
+  <si>
+    <t>0.079457</t>
+  </si>
+  <si>
+    <t>WASTE3</t>
+  </si>
+  <si>
+    <t>0.050002</t>
+  </si>
+  <si>
+    <t>0.069922</t>
+  </si>
+  <si>
+    <t>20.150241</t>
+  </si>
+  <si>
+    <t>73.180896</t>
   </si>
 </sst>
 </file>
@@ -442,13 +556,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D33" sqref="D33:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -478,7 +598,7 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -486,10 +606,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
         <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -497,91 +620,340 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
         <v>11</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
       </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s">
         <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" t="s">
         <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
         <v>19</v>
       </c>
-      <c r="D10" t="s">
-        <v>19</v>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SD works for this iteration! :D
</commit_message>
<xml_diff>
--- a/parsed_scenarios.xlsx
+++ b/parsed_scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oscarste\OneDrive - Chalmers\Local files\Python repos\BECCS-Sweden\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F695184-44BC-47D0-85BD-FCAEC95817D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F385906-E438-45E3-B6D5-349704A1E801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="58215" yWindow="1620" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="124">
   <si>
     <t>Scenario</t>
   </si>
@@ -160,6 +160,9 @@
     <t>80.944133</t>
   </si>
   <si>
+    <t>0.000000e+00</t>
+  </si>
+  <si>
     <t>2.985703</t>
   </si>
   <si>
@@ -175,6 +178,9 @@
     <t>74.087937</t>
   </si>
   <si>
+    <t>0.000000</t>
+  </si>
+  <si>
     <t>0.052697</t>
   </si>
   <si>
@@ -194,13 +200,205 @@
   </si>
   <si>
     <t>73.180896</t>
+  </si>
+  <si>
+    <t>7.565502e-134</t>
+  </si>
+  <si>
+    <t>PULP1</t>
+  </si>
+  <si>
+    <t>20.240774</t>
+  </si>
+  <si>
+    <t>67.783553</t>
+  </si>
+  <si>
+    <t>BarkIncrease</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>SupplyStrategy</t>
+  </si>
+  <si>
+    <t>{SteamLP}  {SteamLP}</t>
+  </si>
+  <si>
+    <t>{SteamLP, SteamHP}  {SteamLP, SteamHP}</t>
+  </si>
+  <si>
+    <t>rate</t>
+  </si>
+  <si>
+    <t>0.865837</t>
+  </si>
+  <si>
+    <t>0.926882</t>
+  </si>
+  <si>
+    <t>PULP2</t>
+  </si>
+  <si>
+    <t>20.119278</t>
+  </si>
+  <si>
+    <t>58.274761</t>
+  </si>
+  <si>
+    <t>30.0</t>
+  </si>
+  <si>
+    <t>45.633321</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>0.600052</t>
+  </si>
+  <si>
+    <t>0.658961</t>
+  </si>
+  <si>
+    <t>1.373677e-23</t>
+  </si>
+  <si>
+    <t>{HeatPumps, SteamLP}  {HeatPumps, SteamLP}</t>
+  </si>
+  <si>
+    <t>PULP3</t>
+  </si>
+  <si>
+    <t>0.818493</t>
+  </si>
+  <si>
+    <t>0.897492</t>
+  </si>
+  <si>
+    <t>20.071454</t>
+  </si>
+  <si>
+    <t>49.940652</t>
+  </si>
+  <si>
+    <t>0.600128</t>
+  </si>
+  <si>
+    <t>0.688997</t>
+  </si>
+  <si>
+    <t>2.769825e-116</t>
+  </si>
+  <si>
+    <t>PULP4</t>
+  </si>
+  <si>
+    <t>{HeatPumps}  {HeatPumps}</t>
+  </si>
+  <si>
+    <t>2.97134</t>
+  </si>
+  <si>
+    <t>3.797015</t>
+  </si>
+  <si>
+    <t>34.16836</t>
+  </si>
+  <si>
+    <t>75.165437</t>
+  </si>
+  <si>
+    <t>20.156281</t>
+  </si>
+  <si>
+    <t>48.59367</t>
+  </si>
+  <si>
+    <t>4.649574e-45</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>-138.037381</t>
+  </si>
+  <si>
+    <t>156.342545</t>
+  </si>
+  <si>
+    <t>PULP5</t>
+  </si>
+  <si>
+    <t>20.21395</t>
+  </si>
+  <si>
+    <t>58.405827</t>
+  </si>
+  <si>
+    <t>1.091327e-25</t>
+  </si>
+  <si>
+    <t>24.253493</t>
+  </si>
+  <si>
+    <t>61.921461</t>
+  </si>
+  <si>
+    <t>0.05608</t>
+  </si>
+  <si>
+    <t>0.112209</t>
+  </si>
+  <si>
+    <t>PULP6</t>
+  </si>
+  <si>
+    <t>20.219613</t>
+  </si>
+  <si>
+    <t>58.340813</t>
+  </si>
+  <si>
+    <t>67.599695</t>
+  </si>
+  <si>
+    <t>0.600147</t>
+  </si>
+  <si>
+    <t>0.664264</t>
+  </si>
+  <si>
+    <t>2.467977e-66</t>
+  </si>
+  <si>
+    <t>PULP7</t>
+  </si>
+  <si>
+    <t>20.190757</t>
+  </si>
+  <si>
+    <t>62.788717</t>
+  </si>
+  <si>
+    <t>67.874617</t>
+  </si>
+  <si>
+    <t>0.820349</t>
+  </si>
+  <si>
+    <t>0.85845</t>
+  </si>
+  <si>
+    <t>1.272422e-18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,6 +410,14 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -249,11 +455,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,18 +764,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33:D34"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="45.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -839,121 +1047,694 @@
         <v>25</v>
       </c>
     </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" t="s">
-        <v>28</v>
+        <v>36</v>
+      </c>
+      <c r="C23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="D24" t="s">
-        <v>47</v>
+        <v>52</v>
+      </c>
+      <c r="E24" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D25" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" t="s">
-        <v>28</v>
+        <v>15</v>
+      </c>
+      <c r="C26" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B27" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="C27" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="D27" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" t="s">
+        <v>66</v>
+      </c>
+      <c r="E33" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" t="s">
+        <v>78</v>
+      </c>
+      <c r="D39" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" t="s">
+        <v>66</v>
+      </c>
+      <c r="D40" t="s">
+        <v>80</v>
+      </c>
+      <c r="E40" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" t="s">
+        <v>85</v>
+      </c>
+      <c r="D44" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>82</v>
+      </c>
+      <c r="B45" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45" t="s">
+        <v>87</v>
+      </c>
+      <c r="D45" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>82</v>
+      </c>
+      <c r="B46" t="s">
+        <v>66</v>
+      </c>
+      <c r="D46" t="s">
+        <v>89</v>
+      </c>
+      <c r="E46" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>90</v>
+      </c>
+      <c r="B50" t="s">
+        <v>36</v>
+      </c>
+      <c r="C50" t="s">
+        <v>96</v>
+      </c>
+      <c r="D50" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>90</v>
+      </c>
+      <c r="B51" t="s">
+        <v>66</v>
+      </c>
+      <c r="D51" t="s">
+        <v>98</v>
+      </c>
+      <c r="E51" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>90</v>
+      </c>
+      <c r="B52" t="s">
+        <v>99</v>
+      </c>
+      <c r="C52" t="s">
+        <v>100</v>
+      </c>
+      <c r="D52" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>102</v>
+      </c>
+      <c r="B56" t="s">
+        <v>66</v>
+      </c>
+      <c r="D56" t="s">
+        <v>105</v>
+      </c>
+      <c r="E56" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>102</v>
+      </c>
+      <c r="B57" t="s">
+        <v>36</v>
+      </c>
+      <c r="C57" t="s">
+        <v>106</v>
+      </c>
+      <c r="D57" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>102</v>
+      </c>
+      <c r="B58" t="s">
         <v>15</v>
       </c>
-      <c r="C28" t="s">
-        <v>54</v>
-      </c>
-      <c r="D28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>53</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="C58" t="s">
+        <v>108</v>
+      </c>
+      <c r="D58" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C29" t="s">
-        <v>56</v>
-      </c>
-      <c r="D29" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" t="s">
-        <v>28</v>
+      <c r="C59" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>110</v>
+      </c>
+      <c r="B62" t="s">
+        <v>36</v>
+      </c>
+      <c r="C62" t="s">
+        <v>111</v>
+      </c>
+      <c r="D62" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>110</v>
+      </c>
+      <c r="B63" t="s">
+        <v>77</v>
+      </c>
+      <c r="C63" t="s">
+        <v>114</v>
+      </c>
+      <c r="D63" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>110</v>
+      </c>
+      <c r="B64" t="s">
+        <v>66</v>
+      </c>
+      <c r="D64" t="s">
+        <v>116</v>
+      </c>
+      <c r="E64" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>117</v>
+      </c>
+      <c r="B68" t="s">
+        <v>36</v>
+      </c>
+      <c r="C68" t="s">
+        <v>118</v>
+      </c>
+      <c r="D68" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>117</v>
+      </c>
+      <c r="B69" t="s">
+        <v>69</v>
+      </c>
+      <c r="C69" t="s">
+        <v>121</v>
+      </c>
+      <c r="D69" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>117</v>
+      </c>
+      <c r="B70" t="s">
+        <v>66</v>
+      </c>
+      <c r="D70" t="s">
+        <v>123</v>
+      </c>
+      <c r="E70" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>